<commit_message>
updated results for model v2
</commit_message>
<xml_diff>
--- a/models/model_logistic_regression_v2/predicted_labels_test_set_v2.xlsx
+++ b/models/model_logistic_regression_v2/predicted_labels_test_set_v2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B59"/>
+  <dimension ref="A1:B60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Sample_0217</t>
+          <t>Sample_0199</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -458,17 +458,17 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Sample_0085</t>
+          <t>Sample_0172</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Sample_0223</t>
+          <t>Sample_0024</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -478,7 +478,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>Sample_0057</t>
+          <t>Sample_0133</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -488,7 +488,7 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Sample_0047</t>
+          <t>Sample_0214</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -498,7 +498,7 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>Sample_0015</t>
+          <t>Sample_0245</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -508,17 +508,17 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>Sample_0012</t>
+          <t>Sample_0123</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>Sample_0015</t>
+          <t>Sample_0106</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -528,7 +528,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Sample_0118</t>
+          <t>Sample_0026</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -538,7 +538,7 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Sample_0117</t>
+          <t>Sample_0229</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -548,7 +548,7 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Sample_0126</t>
+          <t>Sample_0216</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -558,7 +558,7 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>Sample_0221</t>
+          <t>Sample_0023</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -568,7 +568,7 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Sample_0016</t>
+          <t>Sample_0221</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -578,7 +578,7 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Sample_0226</t>
+          <t>Sample_0111</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -588,37 +588,37 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>Sample_0108</t>
+          <t>Sample_0174</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>Sample_0246</t>
+          <t>Sample_0173</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Sample_0220</t>
+          <t>Sample_0205</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Sample_0053</t>
+          <t>Sample_0016</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -628,7 +628,7 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Sample_0230</t>
+          <t>Sample_0128</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -638,7 +638,7 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Sample_0033</t>
+          <t>Sample_0247</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -648,7 +648,7 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>Sample_0024</t>
+          <t>Sample_0171</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -658,7 +658,7 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Sample_0020</t>
+          <t>Sample_0151</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -668,17 +668,17 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Sample_0057</t>
+          <t>Sample_0198</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Sample_0099</t>
+          <t>Sample_0092</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -688,67 +688,67 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>Sample_0062</t>
+          <t>Sample_0143</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>Sample_0108</t>
+          <t>Sample_0120</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Sample_0097</t>
+          <t>Sample_0188</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>Sample_0017</t>
+          <t>Sample_0233</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>Sample_0034</t>
+          <t>Sample_0045</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>Sample_0086</t>
+          <t>Sample_0122</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>Sample_0234</t>
+          <t>Sample_0140</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -758,7 +758,7 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Sample_0062</t>
+          <t>Sample_0179</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -768,7 +768,7 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>Sample_0009</t>
+          <t>Sample_0243</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -778,7 +778,7 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Sample_0122</t>
+          <t>Sample_0035</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -788,7 +788,7 @@
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>Sample_0093</t>
+          <t>Sample_0197</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -798,27 +798,27 @@
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>Sample_0229</t>
+          <t>Sample_0153</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>Sample_0106</t>
+          <t>Sample_0107</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>Sample_0247</t>
+          <t>Sample_0027</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -828,7 +828,7 @@
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>Sample_0251</t>
+          <t>Sample_0182</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -838,67 +838,67 @@
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>Sample_0026</t>
+          <t>Sample_0134</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>Sample_0100</t>
+          <t>Sample_0012</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>Sample_0040</t>
+          <t>Sample_0118</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>Sample_0123</t>
+          <t>Sample_0196</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>Sample_0087</t>
+          <t>Sample_0155</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>Sample_0095</t>
+          <t>Sample_0228</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>Sample_0023</t>
+          <t>Sample_0183</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -908,7 +908,7 @@
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>Sample_0128</t>
+          <t>Sample_0225</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -918,7 +918,7 @@
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>Sample_0038</t>
+          <t>Sample_0019</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -928,7 +928,7 @@
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>Sample_0227</t>
+          <t>Sample_0062</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -938,7 +938,7 @@
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>Sample_0248</t>
+          <t>Sample_0222</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -948,7 +948,7 @@
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>Sample_0024</t>
+          <t>Sample_0089</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -958,17 +958,17 @@
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>Sample_0219</t>
+          <t>Sample_0119</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>Sample_0013</t>
+          <t>Sample_0195</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -978,17 +978,17 @@
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>Sample_0032</t>
+          <t>Sample_0136</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>Sample_0116</t>
+          <t>Sample_0178</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -998,30 +998,40 @@
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>Sample_0044</t>
+          <t>Sample_0184</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>Sample_0112</t>
+          <t>Sample_0044</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>Sample_0111</t>
+          <t>Sample_0192</t>
         </is>
       </c>
       <c r="B59" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="inlineStr">
+        <is>
+          <t>Sample_0230</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>